<commit_message>
Updated project to complete updates.
</commit_message>
<xml_diff>
--- a/Operation_BATO-Doc.xlsx
+++ b/Operation_BATO-Doc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patrick.wylie\Documents\UiPath\OperationBATO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.prado\Documents\GitHub\Operation-BATO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706C4A79-2F80-4CF9-9A37-469FF7D75D2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8EE372-69AB-43BB-A339-E98E0C6446EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E152104B-E930-469F-BC83-3D4F262E677A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E152104B-E930-469F-BC83-3D4F262E677A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,18 +466,18 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" customWidth="1"/>
+    <col min="8" max="8" width="26.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:26" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="57.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -521,7 +521,7 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -547,7 +547,7 @@
         <v>43763</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -573,7 +573,7 @@
         <v>43764</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -599,7 +599,7 @@
         <v>43765</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -625,7 +625,7 @@
         <v>43766</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -651,7 +651,7 @@
         <v>43767</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -679,8 +679,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" display="https://afs365.sharepoint.com/:x:/r/sites/SADC-RPAKickoff/Shared Documents/General/Testing Folder/Operation BATO/Master TTEC Agency ATO Tracker Demo.xlsx?d=wf8b81b86595c49829f1bad7b63d26591&amp;csf=1&amp;e=ePSM8X" xr:uid="{DD2EA7EE-9033-4B73-A68C-251FA4D4C083}"/>
-    <hyperlink ref="G6" r:id="rId2" display="https://afs365.sharepoint.com/:x:/r/sites/SADC-RPAKickoff/Shared Documents/General/Testing Folder/Operation BATO/Master TTEC Agency ATO Tracker Demo.xlsx?d=wf8b81b86595c49829f1bad7b63d26591&amp;csf=1&amp;e=amDnFE" xr:uid="{6AECA202-095E-43FB-890B-2F89B995C427}"/>
+    <hyperlink ref="G5" r:id="rId1" display="https://afs365.sharepoint.com/:x:/r/sites/SADC-RPAKickoff/Shared Documents/General/Testing Folder/Operation BATO/Master TTEC Agency ATO Tracker Demo.xlsx" xr:uid="{DD2EA7EE-9033-4B73-A68C-251FA4D4C083}"/>
+    <hyperlink ref="G6" r:id="rId2" display="https://afs365.sharepoint.com/:x:/r/sites/SADC-RPAKickoff/Shared Documents/General/Testing Folder/Operation BATO/Master TTEC Agency ATO Tracker Demo1.xlsx" xr:uid="{6AECA202-095E-43FB-890B-2F89B995C427}"/>
     <hyperlink ref="G7" r:id="rId3" display="https://afs365.sharepoint.com/:x:/r/sites/SADC-RPAKickoff/Shared Documents/General/Testing Folder/Operation BATO/Master TTEC Agency ATO Tracker Demo2.xlsx" xr:uid="{5C23666B-BA1F-48D7-884D-FCED1A580EDE}"/>
     <hyperlink ref="G8" r:id="rId4" display="https://afs365.sharepoint.com/:x:/r/sites/SADC-RPAKickoff/Shared Documents/General/Testing Folder/Operation BATO/Master TTEC Agency ATO Tracker Demo3.xlsx" xr:uid="{241CD651-BC07-4CD3-8D9A-562AEFC86C94}"/>
     <hyperlink ref="G9" r:id="rId5" display="https://afs365.sharepoint.com/:x:/r/sites/SADC-RPAKickoff/Shared Documents/General/Testing Folder/Operation BATO/Master TTEC Agency ATO Tracker Demo4.xlsx" xr:uid="{87D4139F-D7BF-44F5-ACE7-4EA77C260AAF}"/>

</xml_diff>